<commit_message>
Add new counter for RAD Geiger detector
Temporary detector for RAD evaluation tests.
IP: 10.128.115.227
Device is connected to channel #04
</commit_message>
<xml_diff>
--- a/scripts/spreadsheet/Redes e Beaglebones.xlsx
+++ b/scripts/spreadsheet/Redes e Beaglebones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cnpemcamp.sharepoint.com/sites/controle/Documentos Compartilhados/Redes e Beaglebones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F03F25-A2C1-4006-808C-63DF8CB3C3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4870B997-A2C8-43D1-88A3-C6C2110FC98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="990" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="990" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="23" r:id="rId1"/>
@@ -30,10 +30,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PVs MBTemp'!$A$1:$N$196</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'PVs RackMonitoring'!$A$1:$M$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'PVs Counting PRU'!$A$1:$X$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'PVs Counting PRU'!$A$1:$X$81</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -41,6 +44,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -51,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7686" uniqueCount="2282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7702" uniqueCount="2282">
   <si>
     <t>ENABLE</t>
   </si>
@@ -14783,11 +14788,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EA83DB-34C0-457B-9236-8486C04FD179}">
-  <dimension ref="A1:AB80"/>
+  <dimension ref="A1:AB81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="M60" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="U62" sqref="U62"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -14797,7 +14802,14 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="7.140625" style="65" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="12" width="38.140625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="12" max="12" width="38.140625" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" customWidth="1"/>
     <col min="15" max="15" width="20.85546875" customWidth="1"/>
@@ -20733,52 +20745,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="62" spans="1:28" hidden="1">
+    <row r="62" spans="1:28">
       <c r="A62" s="93" t="s">
-        <v>1046</v>
+        <v>30</v>
       </c>
       <c r="B62" t="str">
-        <f>_xlfn.CONCAT("10.128.",C62 + 100,".151")</f>
-        <v>10.128.116.151</v>
+        <f>_xlfn.CONCAT("10.128.",C62 + 100,".227")</f>
+        <v>10.128.115.227</v>
       </c>
       <c r="C62" s="65">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D62" t="str">
-        <f>_xlfn.CONCAT("SI-",C62,"M2:CO-Counter")</f>
-        <v>SI-16M2:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C62,"xx:CO-Counter")</f>
+        <v>SI-15xx:CO-Counter</v>
       </c>
       <c r="E62" s="40" t="str">
-        <f>_xlfn.CONCAT($D62,":Ch1")</f>
-        <v>SI-16M2:CO-Counter:Ch1</v>
+        <f>_xlfn.CONCAT($D62,"-Ch1")</f>
+        <v>SI-15xx:CO-Counter-Ch1</v>
       </c>
       <c r="F62" s="40" t="str">
         <f>_xlfn.CONCAT($D62,"-Ch2")</f>
-        <v>SI-16M2:CO-Counter-Ch2</v>
+        <v>SI-15xx:CO-Counter-Ch2</v>
       </c>
       <c r="G62" s="40" t="str">
         <f>_xlfn.CONCAT($D62,"-Ch3")</f>
-        <v>SI-16M2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H62" s="40" t="str">
-        <f>_xlfn.CONCAT($D62,":Ch4")</f>
-        <v>SI-16M2:CO-Counter:Ch4</v>
+        <v>SI-15xx:CO-Counter-Ch3</v>
+      </c>
+      <c r="H62" t="str">
+        <f>_xlfn.CONCAT("RAD:GMC:Geiger")</f>
+        <v>RAD:GMC:Geiger</v>
       </c>
       <c r="I62" s="40" t="str">
         <f>_xlfn.CONCAT($D62,"-Ch5")</f>
-        <v>SI-16M2:CO-Counter-Ch5</v>
+        <v>SI-15xx:CO-Counter-Ch5</v>
       </c>
       <c r="J62" s="40" t="str">
         <f>_xlfn.CONCAT($D62,"-Ch6")</f>
-        <v>SI-16M2:CO-Counter-Ch6</v>
+        <v>SI-15xx:CO-Counter-Ch6</v>
       </c>
       <c r="K62" s="40" t="str">
         <f>_xlfn.CONCAT($D62,"-Ch7")</f>
-        <v>SI-16M2:CO-Counter-Ch7</v>
+        <v>SI-15xx:CO-Counter-Ch7</v>
       </c>
       <c r="L62" s="40" t="str">
         <f>_xlfn.CONCAT($D62,"-Ch8")</f>
-        <v>SI-16M2:CO-Counter-Ch8</v>
+        <v>SI-15xx:CO-Counter-Ch8</v>
       </c>
       <c r="M62" t="s">
         <v>2090</v>
@@ -20804,7 +20816,7 @@
       <c r="T62" t="s">
         <v>2097</v>
       </c>
-      <c r="U62" t="s">
+      <c r="U62" s="40" t="s">
         <v>2098</v>
       </c>
       <c r="V62" t="s">
@@ -20813,8 +20825,9 @@
       <c r="W62" t="s">
         <v>2098</v>
       </c>
-      <c r="X62" t="s">
-        <v>2098</v>
+      <c r="X62" t="str">
+        <f>_xlfn.CONCAT("RAD:GMC:Geiger")</f>
+        <v>RAD:GMC:Geiger</v>
       </c>
       <c r="Y62" t="s">
         <v>2098</v>
@@ -20831,50 +20844,50 @@
     </row>
     <row r="63" spans="1:28">
       <c r="A63" s="93" t="s">
-        <v>30</v>
+        <v>1046</v>
       </c>
       <c r="B63" t="str">
-        <f>_xlfn.CONCAT("10.128.",C63 + 100,".152")</f>
-        <v>10.128.116.152</v>
+        <f>_xlfn.CONCAT("10.128.",C63 + 100,".151")</f>
+        <v>10.128.116.151</v>
       </c>
       <c r="C63" s="65">
         <v>16</v>
       </c>
       <c r="D63" t="str">
-        <f>_xlfn.CONCAT("SI-",C63,"C2:CO-Counter")</f>
-        <v>SI-16C2:CO-Counter</v>
-      </c>
-      <c r="E63" t="str">
-        <f>_xlfn.CONCAT("SI-",$C63,"M2:CO-Gamma")</f>
-        <v>SI-16M2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",C63,"M2:CO-Counter")</f>
+        <v>SI-16M2:CO-Counter</v>
+      </c>
+      <c r="E63" s="40" t="str">
+        <f>_xlfn.CONCAT($D63,":Ch1")</f>
+        <v>SI-16M2:CO-Counter:Ch1</v>
       </c>
       <c r="F63" s="40" t="str">
         <f>_xlfn.CONCAT($D63,"-Ch2")</f>
-        <v>SI-16C2:CO-Counter-Ch2</v>
+        <v>SI-16M2:CO-Counter-Ch2</v>
       </c>
       <c r="G63" s="40" t="str">
         <f>_xlfn.CONCAT($D63,"-Ch3")</f>
-        <v>SI-16C2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H63" t="str">
-        <f>_xlfn.CONCAT("SI-",$C63,"C1:CO-Gamma")</f>
-        <v>SI-16C1:CO-Gamma</v>
+        <v>SI-16M2:CO-Counter-Ch3</v>
+      </c>
+      <c r="H63" s="40" t="str">
+        <f>_xlfn.CONCAT($D63,":Ch4")</f>
+        <v>SI-16M2:CO-Counter:Ch4</v>
       </c>
       <c r="I63" s="40" t="str">
         <f>_xlfn.CONCAT($D63,"-Ch5")</f>
-        <v>SI-16C2:CO-Counter-Ch5</v>
+        <v>SI-16M2:CO-Counter-Ch5</v>
       </c>
       <c r="J63" s="40" t="str">
         <f>_xlfn.CONCAT($D63,"-Ch6")</f>
-        <v>SI-16C2:CO-Counter-Ch6</v>
+        <v>SI-16M2:CO-Counter-Ch6</v>
       </c>
       <c r="K63" s="40" t="str">
         <f>_xlfn.CONCAT($D63,"-Ch7")</f>
-        <v>SI-16C2:CO-Counter-Ch7</v>
+        <v>SI-16M2:CO-Counter-Ch7</v>
       </c>
       <c r="L63" s="40" t="str">
         <f>_xlfn.CONCAT($D63,"-Ch8")</f>
-        <v>SI-16C2:CO-Counter-Ch8</v>
+        <v>SI-16M2:CO-Counter-Ch8</v>
       </c>
       <c r="M63" t="s">
         <v>2090</v>
@@ -20900,9 +20913,8 @@
       <c r="T63" t="s">
         <v>2097</v>
       </c>
-      <c r="U63" t="str">
-        <f>_xlfn.CONCAT("SI-",$C63,"C1:CO-GammaDetector")</f>
-        <v>SI-16C1:CO-GammaDetector</v>
+      <c r="U63" t="s">
+        <v>2098</v>
       </c>
       <c r="V63" t="s">
         <v>2098</v>
@@ -20910,9 +20922,8 @@
       <c r="W63" t="s">
         <v>2098</v>
       </c>
-      <c r="X63" t="str">
-        <f>_xlfn.CONCAT("SI-",$C63,"C2:CO-GammaDetector")</f>
-        <v>SI-16C2:CO-GammaDetector</v>
+      <c r="X63" t="s">
+        <v>2098</v>
       </c>
       <c r="Y63" t="s">
         <v>2098</v>
@@ -20932,47 +20943,47 @@
         <v>30</v>
       </c>
       <c r="B64" t="str">
-        <f>_xlfn.CONCAT("10.128.",C64 + 100,".153")</f>
-        <v>10.128.116.153</v>
+        <f>_xlfn.CONCAT("10.128.",C64 + 100,".152")</f>
+        <v>10.128.116.152</v>
       </c>
       <c r="C64" s="65">
         <v>16</v>
       </c>
       <c r="D64" t="str">
-        <f>_xlfn.CONCAT("SI-",C64,"C3:CO-Counter")</f>
-        <v>SI-16C3:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C64,"C2:CO-Counter")</f>
+        <v>SI-16C2:CO-Counter</v>
       </c>
       <c r="E64" t="str">
-        <f>_xlfn.CONCAT("SI-",$C64,"C2:CO-Gamma")</f>
-        <v>SI-16C2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C64,"M2:CO-Gamma")</f>
+        <v>SI-16M2:CO-Gamma</v>
       </c>
       <c r="F64" s="40" t="str">
         <f>_xlfn.CONCAT($D64,"-Ch2")</f>
-        <v>SI-16C3:CO-Counter-Ch2</v>
+        <v>SI-16C2:CO-Counter-Ch2</v>
       </c>
       <c r="G64" s="40" t="str">
         <f>_xlfn.CONCAT($D64,"-Ch3")</f>
-        <v>SI-16C3:CO-Counter-Ch3</v>
+        <v>SI-16C2:CO-Counter-Ch3</v>
       </c>
       <c r="H64" t="str">
-        <f>_xlfn.CONCAT("SI-",$C64,"C3:CO-Gamma")</f>
-        <v>SI-16C3:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C64,"C1:CO-Gamma")</f>
+        <v>SI-16C1:CO-Gamma</v>
       </c>
       <c r="I64" s="40" t="str">
         <f>_xlfn.CONCAT($D64,"-Ch5")</f>
-        <v>SI-16C3:CO-Counter-Ch5</v>
+        <v>SI-16C2:CO-Counter-Ch5</v>
       </c>
       <c r="J64" s="40" t="str">
         <f>_xlfn.CONCAT($D64,"-Ch6")</f>
-        <v>SI-16C3:CO-Counter-Ch6</v>
+        <v>SI-16C2:CO-Counter-Ch6</v>
       </c>
       <c r="K64" s="40" t="str">
         <f>_xlfn.CONCAT($D64,"-Ch7")</f>
-        <v>SI-16C3:CO-Counter-Ch7</v>
+        <v>SI-16C2:CO-Counter-Ch7</v>
       </c>
       <c r="L64" s="40" t="str">
         <f>_xlfn.CONCAT($D64,"-Ch8")</f>
-        <v>SI-16C3:CO-Counter-Ch8</v>
+        <v>SI-16C2:CO-Counter-Ch8</v>
       </c>
       <c r="M64" t="s">
         <v>2090</v>
@@ -20999,8 +21010,8 @@
         <v>2097</v>
       </c>
       <c r="U64" t="str">
-        <f>_xlfn.CONCAT("SI-",$C64,"C3:CO-GammaDetector")</f>
-        <v>SI-16C3:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C64,"C1:CO-GammaDetector")</f>
+        <v>SI-16C1:CO-GammaDetector</v>
       </c>
       <c r="V64" t="s">
         <v>2098</v>
@@ -21009,8 +21020,8 @@
         <v>2098</v>
       </c>
       <c r="X64" t="str">
-        <f>_xlfn.CONCAT("SI-",$C64,"C4:CO-GammaDetector")</f>
-        <v>SI-16C4:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C64,"C2:CO-GammaDetector")</f>
+        <v>SI-16C2:CO-GammaDetector</v>
       </c>
       <c r="Y64" t="s">
         <v>2098</v>
@@ -21030,47 +21041,47 @@
         <v>30</v>
       </c>
       <c r="B65" t="str">
-        <f>_xlfn.CONCAT("10.128.",C65 + 100,".154")</f>
-        <v>10.128.116.154</v>
+        <f>_xlfn.CONCAT("10.128.",C65 + 100,".153")</f>
+        <v>10.128.116.153</v>
       </c>
       <c r="C65" s="65">
         <v>16</v>
       </c>
       <c r="D65" t="str">
-        <f>_xlfn.CONCAT("SI-",C65+1,"M1:CO-Counter")</f>
-        <v>SI-17M1:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C65,"C3:CO-Counter")</f>
+        <v>SI-16C3:CO-Counter</v>
       </c>
       <c r="E65" t="str">
-        <f>_xlfn.CONCAT("SI-",$C65,"C4:CO-Gamma")</f>
-        <v>SI-16C4:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C65,"C2:CO-Gamma")</f>
+        <v>SI-16C2:CO-Gamma</v>
       </c>
       <c r="F65" s="40" t="str">
         <f>_xlfn.CONCAT($D65,"-Ch2")</f>
-        <v>SI-17M1:CO-Counter-Ch2</v>
+        <v>SI-16C3:CO-Counter-Ch2</v>
       </c>
       <c r="G65" s="40" t="str">
         <f>_xlfn.CONCAT($D65,"-Ch3")</f>
-        <v>SI-17M1:CO-Counter-Ch3</v>
-      </c>
-      <c r="H65" s="135" t="str">
-        <f>_xlfn.CONCAT($D65,"-Ch4")</f>
-        <v>SI-17M1:CO-Counter-Ch4</v>
+        <v>SI-16C3:CO-Counter-Ch3</v>
+      </c>
+      <c r="H65" t="str">
+        <f>_xlfn.CONCAT("SI-",$C65,"C3:CO-Gamma")</f>
+        <v>SI-16C3:CO-Gamma</v>
       </c>
       <c r="I65" s="40" t="str">
         <f>_xlfn.CONCAT($D65,"-Ch5")</f>
-        <v>SI-17M1:CO-Counter-Ch5</v>
+        <v>SI-16C3:CO-Counter-Ch5</v>
       </c>
       <c r="J65" s="40" t="str">
         <f>_xlfn.CONCAT($D65,"-Ch6")</f>
-        <v>SI-17M1:CO-Counter-Ch6</v>
+        <v>SI-16C3:CO-Counter-Ch6</v>
       </c>
       <c r="K65" s="40" t="str">
         <f>_xlfn.CONCAT($D65,"-Ch7")</f>
-        <v>SI-17M1:CO-Counter-Ch7</v>
+        <v>SI-16C3:CO-Counter-Ch7</v>
       </c>
       <c r="L65" s="40" t="str">
         <f>_xlfn.CONCAT($D65,"-Ch8")</f>
-        <v>SI-17M1:CO-Counter-Ch8</v>
+        <v>SI-16C3:CO-Counter-Ch8</v>
       </c>
       <c r="M65" t="s">
         <v>2090</v>
@@ -21097,8 +21108,8 @@
         <v>2097</v>
       </c>
       <c r="U65" t="str">
-        <f>_xlfn.CONCAT("SI-",$C65+1,"M1:CO-GammaDetector")</f>
-        <v>SI-17M1:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C65,"C3:CO-GammaDetector")</f>
+        <v>SI-16C3:CO-GammaDetector</v>
       </c>
       <c r="V65" t="s">
         <v>2098</v>
@@ -21106,8 +21117,9 @@
       <c r="W65" t="s">
         <v>2098</v>
       </c>
-      <c r="X65" s="40" t="s">
-        <v>2098</v>
+      <c r="X65" t="str">
+        <f>_xlfn.CONCAT("SI-",$C65,"C4:CO-GammaDetector")</f>
+        <v>SI-16C4:CO-GammaDetector</v>
       </c>
       <c r="Y65" t="s">
         <v>2098</v>
@@ -21122,52 +21134,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="66" spans="1:28" hidden="1">
+    <row r="66" spans="1:28">
       <c r="A66" s="93" t="s">
-        <v>1046</v>
+        <v>30</v>
       </c>
       <c r="B66" t="str">
-        <f>_xlfn.CONCAT("10.128.",C66 + 100,".151")</f>
-        <v>10.128.117.151</v>
+        <f>_xlfn.CONCAT("10.128.",C66 + 100,".154")</f>
+        <v>10.128.116.154</v>
       </c>
       <c r="C66" s="65">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" t="str">
-        <f>_xlfn.CONCAT("SI-",C66,"M2:CO-Counter")</f>
-        <v>SI-17M2:CO-Counter</v>
-      </c>
-      <c r="E66" s="40" t="str">
-        <f>_xlfn.CONCAT($D66,":Ch1")</f>
-        <v>SI-17M2:CO-Counter:Ch1</v>
+        <f>_xlfn.CONCAT("SI-",C66+1,"M1:CO-Counter")</f>
+        <v>SI-17M1:CO-Counter</v>
+      </c>
+      <c r="E66" t="str">
+        <f>_xlfn.CONCAT("SI-",$C66,"C4:CO-Gamma")</f>
+        <v>SI-16C4:CO-Gamma</v>
       </c>
       <c r="F66" s="40" t="str">
         <f>_xlfn.CONCAT($D66,"-Ch2")</f>
-        <v>SI-17M2:CO-Counter-Ch2</v>
+        <v>SI-17M1:CO-Counter-Ch2</v>
       </c>
       <c r="G66" s="40" t="str">
         <f>_xlfn.CONCAT($D66,"-Ch3")</f>
-        <v>SI-17M2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H66" s="40" t="str">
-        <f>_xlfn.CONCAT($D66,":Ch4")</f>
-        <v>SI-17M2:CO-Counter:Ch4</v>
+        <v>SI-17M1:CO-Counter-Ch3</v>
+      </c>
+      <c r="H66" s="135" t="str">
+        <f>_xlfn.CONCAT($D66,"-Ch4")</f>
+        <v>SI-17M1:CO-Counter-Ch4</v>
       </c>
       <c r="I66" s="40" t="str">
         <f>_xlfn.CONCAT($D66,"-Ch5")</f>
-        <v>SI-17M2:CO-Counter-Ch5</v>
+        <v>SI-17M1:CO-Counter-Ch5</v>
       </c>
       <c r="J66" s="40" t="str">
         <f>_xlfn.CONCAT($D66,"-Ch6")</f>
-        <v>SI-17M2:CO-Counter-Ch6</v>
+        <v>SI-17M1:CO-Counter-Ch6</v>
       </c>
       <c r="K66" s="40" t="str">
         <f>_xlfn.CONCAT($D66,"-Ch7")</f>
-        <v>SI-17M2:CO-Counter-Ch7</v>
+        <v>SI-17M1:CO-Counter-Ch7</v>
       </c>
       <c r="L66" s="40" t="str">
         <f>_xlfn.CONCAT($D66,"-Ch8")</f>
-        <v>SI-17M2:CO-Counter-Ch8</v>
+        <v>SI-17M1:CO-Counter-Ch8</v>
       </c>
       <c r="M66" t="s">
         <v>2090</v>
@@ -21193,8 +21205,9 @@
       <c r="T66" t="s">
         <v>2097</v>
       </c>
-      <c r="U66" t="s">
-        <v>2098</v>
+      <c r="U66" t="str">
+        <f>_xlfn.CONCAT("SI-",$C66+1,"M1:CO-GammaDetector")</f>
+        <v>SI-17M1:CO-GammaDetector</v>
       </c>
       <c r="V66" t="s">
         <v>2098</v>
@@ -21202,7 +21215,7 @@
       <c r="W66" t="s">
         <v>2098</v>
       </c>
-      <c r="X66" t="s">
+      <c r="X66" s="40" t="s">
         <v>2098</v>
       </c>
       <c r="Y66" t="s">
@@ -21218,52 +21231,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="67" spans="1:28">
+    <row r="67" spans="1:28" hidden="1">
       <c r="A67" s="93" t="s">
-        <v>30</v>
+        <v>1046</v>
       </c>
       <c r="B67" t="str">
-        <f>_xlfn.CONCAT("10.128.",C67 + 100,".152")</f>
-        <v>10.128.117.152</v>
+        <f>_xlfn.CONCAT("10.128.",C67 + 100,".151")</f>
+        <v>10.128.117.151</v>
       </c>
       <c r="C67" s="65">
         <v>17</v>
       </c>
       <c r="D67" t="str">
-        <f>_xlfn.CONCAT("SI-",C67,"C2:CO-Counter")</f>
-        <v>SI-17C2:CO-Counter</v>
-      </c>
-      <c r="E67" t="str">
-        <f>_xlfn.CONCAT("SI-",$C67,"M2:CO-Gamma")</f>
-        <v>SI-17M2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",C67,"M2:CO-Counter")</f>
+        <v>SI-17M2:CO-Counter</v>
+      </c>
+      <c r="E67" s="40" t="str">
+        <f>_xlfn.CONCAT($D67,":Ch1")</f>
+        <v>SI-17M2:CO-Counter:Ch1</v>
       </c>
       <c r="F67" s="40" t="str">
         <f>_xlfn.CONCAT($D67,"-Ch2")</f>
-        <v>SI-17C2:CO-Counter-Ch2</v>
+        <v>SI-17M2:CO-Counter-Ch2</v>
       </c>
       <c r="G67" s="40" t="str">
         <f>_xlfn.CONCAT($D67,"-Ch3")</f>
-        <v>SI-17C2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H67" t="str">
-        <f>_xlfn.CONCAT("SI-",$C67,"C1:CO-Gamma")</f>
-        <v>SI-17C1:CO-Gamma</v>
+        <v>SI-17M2:CO-Counter-Ch3</v>
+      </c>
+      <c r="H67" s="40" t="str">
+        <f>_xlfn.CONCAT($D67,":Ch4")</f>
+        <v>SI-17M2:CO-Counter:Ch4</v>
       </c>
       <c r="I67" s="40" t="str">
         <f>_xlfn.CONCAT($D67,"-Ch5")</f>
-        <v>SI-17C2:CO-Counter-Ch5</v>
+        <v>SI-17M2:CO-Counter-Ch5</v>
       </c>
       <c r="J67" s="40" t="str">
         <f>_xlfn.CONCAT($D67,"-Ch6")</f>
-        <v>SI-17C2:CO-Counter-Ch6</v>
+        <v>SI-17M2:CO-Counter-Ch6</v>
       </c>
       <c r="K67" s="40" t="str">
         <f>_xlfn.CONCAT($D67,"-Ch7")</f>
-        <v>SI-17C2:CO-Counter-Ch7</v>
+        <v>SI-17M2:CO-Counter-Ch7</v>
       </c>
       <c r="L67" s="40" t="str">
         <f>_xlfn.CONCAT($D67,"-Ch8")</f>
-        <v>SI-17C2:CO-Counter-Ch8</v>
+        <v>SI-17M2:CO-Counter-Ch8</v>
       </c>
       <c r="M67" t="s">
         <v>2090</v>
@@ -21289,9 +21302,8 @@
       <c r="T67" t="s">
         <v>2097</v>
       </c>
-      <c r="U67" t="str">
-        <f>_xlfn.CONCAT("SI-",$C67,"C1:CO-GammaDetector")</f>
-        <v>SI-17C1:CO-GammaDetector</v>
+      <c r="U67" t="s">
+        <v>2098</v>
       </c>
       <c r="V67" t="s">
         <v>2098</v>
@@ -21299,9 +21311,8 @@
       <c r="W67" t="s">
         <v>2098</v>
       </c>
-      <c r="X67" t="str">
-        <f>_xlfn.CONCAT("SI-",$C67,"C2:CO-GammaDetector")</f>
-        <v>SI-17C2:CO-GammaDetector</v>
+      <c r="X67" t="s">
+        <v>2098</v>
       </c>
       <c r="Y67" t="s">
         <v>2098</v>
@@ -21321,47 +21332,47 @@
         <v>30</v>
       </c>
       <c r="B68" t="str">
-        <f>_xlfn.CONCAT("10.128.",C68 + 100,".153")</f>
-        <v>10.128.117.153</v>
+        <f>_xlfn.CONCAT("10.128.",C68 + 100,".152")</f>
+        <v>10.128.117.152</v>
       </c>
       <c r="C68" s="65">
         <v>17</v>
       </c>
       <c r="D68" t="str">
-        <f>_xlfn.CONCAT("SI-",C68,"C3:CO-Counter")</f>
-        <v>SI-17C3:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C68,"C2:CO-Counter")</f>
+        <v>SI-17C2:CO-Counter</v>
       </c>
       <c r="E68" t="str">
-        <f>_xlfn.CONCAT("SI-",$C68,"C2:CO-Gamma")</f>
-        <v>SI-17C2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C68,"M2:CO-Gamma")</f>
+        <v>SI-17M2:CO-Gamma</v>
       </c>
       <c r="F68" s="40" t="str">
         <f>_xlfn.CONCAT($D68,"-Ch2")</f>
-        <v>SI-17C3:CO-Counter-Ch2</v>
+        <v>SI-17C2:CO-Counter-Ch2</v>
       </c>
       <c r="G68" s="40" t="str">
         <f>_xlfn.CONCAT($D68,"-Ch3")</f>
-        <v>SI-17C3:CO-Counter-Ch3</v>
+        <v>SI-17C2:CO-Counter-Ch3</v>
       </c>
       <c r="H68" t="str">
-        <f>_xlfn.CONCAT("SI-",$C68,"C3:CO-Gamma")</f>
-        <v>SI-17C3:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C68,"C1:CO-Gamma")</f>
+        <v>SI-17C1:CO-Gamma</v>
       </c>
       <c r="I68" s="40" t="str">
         <f>_xlfn.CONCAT($D68,"-Ch5")</f>
-        <v>SI-17C3:CO-Counter-Ch5</v>
+        <v>SI-17C2:CO-Counter-Ch5</v>
       </c>
       <c r="J68" s="40" t="str">
         <f>_xlfn.CONCAT($D68,"-Ch6")</f>
-        <v>SI-17C3:CO-Counter-Ch6</v>
+        <v>SI-17C2:CO-Counter-Ch6</v>
       </c>
       <c r="K68" s="40" t="str">
         <f>_xlfn.CONCAT($D68,"-Ch7")</f>
-        <v>SI-17C3:CO-Counter-Ch7</v>
+        <v>SI-17C2:CO-Counter-Ch7</v>
       </c>
       <c r="L68" s="40" t="str">
         <f>_xlfn.CONCAT($D68,"-Ch8")</f>
-        <v>SI-17C3:CO-Counter-Ch8</v>
+        <v>SI-17C2:CO-Counter-Ch8</v>
       </c>
       <c r="M68" t="s">
         <v>2090</v>
@@ -21388,8 +21399,8 @@
         <v>2097</v>
       </c>
       <c r="U68" t="str">
-        <f>_xlfn.CONCAT("SI-",$C68,"C3:CO-GammaDetector")</f>
-        <v>SI-17C3:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C68,"C1:CO-GammaDetector")</f>
+        <v>SI-17C1:CO-GammaDetector</v>
       </c>
       <c r="V68" t="s">
         <v>2098</v>
@@ -21398,8 +21409,8 @@
         <v>2098</v>
       </c>
       <c r="X68" t="str">
-        <f>_xlfn.CONCAT("SI-",$C68,"C4:CO-GammaDetector")</f>
-        <v>SI-17C4:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C68,"C2:CO-GammaDetector")</f>
+        <v>SI-17C2:CO-GammaDetector</v>
       </c>
       <c r="Y68" t="s">
         <v>2098</v>
@@ -21419,47 +21430,47 @@
         <v>30</v>
       </c>
       <c r="B69" t="str">
-        <f>_xlfn.CONCAT("10.128.",C69 + 100,".154")</f>
-        <v>10.128.117.154</v>
+        <f>_xlfn.CONCAT("10.128.",C69 + 100,".153")</f>
+        <v>10.128.117.153</v>
       </c>
       <c r="C69" s="65">
         <v>17</v>
       </c>
       <c r="D69" t="str">
-        <f>_xlfn.CONCAT("SI-",C69+1,"M1:CO-Counter")</f>
-        <v>SI-18M1:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C69,"C3:CO-Counter")</f>
+        <v>SI-17C3:CO-Counter</v>
       </c>
       <c r="E69" t="str">
-        <f>_xlfn.CONCAT("SI-",$C69,"C4:CO-Gamma")</f>
-        <v>SI-17C4:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C69,"C2:CO-Gamma")</f>
+        <v>SI-17C2:CO-Gamma</v>
       </c>
       <c r="F69" s="40" t="str">
         <f>_xlfn.CONCAT($D69,"-Ch2")</f>
-        <v>SI-18M1:CO-Counter-Ch2</v>
+        <v>SI-17C3:CO-Counter-Ch2</v>
       </c>
       <c r="G69" s="40" t="str">
         <f>_xlfn.CONCAT($D69,"-Ch3")</f>
-        <v>SI-18M1:CO-Counter-Ch3</v>
-      </c>
-      <c r="H69" s="40" t="str">
-        <f>_xlfn.CONCAT($D69,"-Ch4")</f>
-        <v>SI-18M1:CO-Counter-Ch4</v>
+        <v>SI-17C3:CO-Counter-Ch3</v>
+      </c>
+      <c r="H69" t="str">
+        <f>_xlfn.CONCAT("SI-",$C69,"C3:CO-Gamma")</f>
+        <v>SI-17C3:CO-Gamma</v>
       </c>
       <c r="I69" s="40" t="str">
         <f>_xlfn.CONCAT($D69,"-Ch5")</f>
-        <v>SI-18M1:CO-Counter-Ch5</v>
+        <v>SI-17C3:CO-Counter-Ch5</v>
       </c>
       <c r="J69" s="40" t="str">
         <f>_xlfn.CONCAT($D69,"-Ch6")</f>
-        <v>SI-18M1:CO-Counter-Ch6</v>
+        <v>SI-17C3:CO-Counter-Ch6</v>
       </c>
       <c r="K69" s="40" t="str">
         <f>_xlfn.CONCAT($D69,"-Ch7")</f>
-        <v>SI-18M1:CO-Counter-Ch7</v>
+        <v>SI-17C3:CO-Counter-Ch7</v>
       </c>
       <c r="L69" s="40" t="str">
         <f>_xlfn.CONCAT($D69,"-Ch8")</f>
-        <v>SI-18M1:CO-Counter-Ch8</v>
+        <v>SI-17C3:CO-Counter-Ch8</v>
       </c>
       <c r="M69" t="s">
         <v>2090</v>
@@ -21486,8 +21497,8 @@
         <v>2097</v>
       </c>
       <c r="U69" t="str">
-        <f>_xlfn.CONCAT("SI-",$C69+1,"M1:CO-GammaDetector")</f>
-        <v>SI-18M1:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C69,"C3:CO-GammaDetector")</f>
+        <v>SI-17C3:CO-GammaDetector</v>
       </c>
       <c r="V69" t="s">
         <v>2098</v>
@@ -21495,8 +21506,9 @@
       <c r="W69" t="s">
         <v>2098</v>
       </c>
-      <c r="X69" s="40" t="s">
-        <v>2098</v>
+      <c r="X69" t="str">
+        <f>_xlfn.CONCAT("SI-",$C69,"C4:CO-GammaDetector")</f>
+        <v>SI-17C4:CO-GammaDetector</v>
       </c>
       <c r="Y69" t="s">
         <v>2098</v>
@@ -21511,52 +21523,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="70" spans="1:28" hidden="1">
+    <row r="70" spans="1:28">
       <c r="A70" s="93" t="s">
-        <v>1046</v>
+        <v>30</v>
       </c>
       <c r="B70" t="str">
-        <f>_xlfn.CONCAT("10.128.",C70 + 100,".151")</f>
-        <v>10.128.118.151</v>
+        <f>_xlfn.CONCAT("10.128.",C70 + 100,".154")</f>
+        <v>10.128.117.154</v>
       </c>
       <c r="C70" s="65">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" t="str">
-        <f>_xlfn.CONCAT("SI-",C70,"M2:CO-Counter")</f>
-        <v>SI-18M2:CO-Counter</v>
-      </c>
-      <c r="E70" s="40" t="str">
-        <f>_xlfn.CONCAT($D70,":Ch1")</f>
-        <v>SI-18M2:CO-Counter:Ch1</v>
+        <f>_xlfn.CONCAT("SI-",C70+1,"M1:CO-Counter")</f>
+        <v>SI-18M1:CO-Counter</v>
+      </c>
+      <c r="E70" t="str">
+        <f>_xlfn.CONCAT("SI-",$C70,"C4:CO-Gamma")</f>
+        <v>SI-17C4:CO-Gamma</v>
       </c>
       <c r="F70" s="40" t="str">
         <f>_xlfn.CONCAT($D70,"-Ch2")</f>
-        <v>SI-18M2:CO-Counter-Ch2</v>
+        <v>SI-18M1:CO-Counter-Ch2</v>
       </c>
       <c r="G70" s="40" t="str">
         <f>_xlfn.CONCAT($D70,"-Ch3")</f>
-        <v>SI-18M2:CO-Counter-Ch3</v>
+        <v>SI-18M1:CO-Counter-Ch3</v>
       </c>
       <c r="H70" s="40" t="str">
-        <f>_xlfn.CONCAT($D70,":Ch4")</f>
-        <v>SI-18M2:CO-Counter:Ch4</v>
+        <f>_xlfn.CONCAT($D70,"-Ch4")</f>
+        <v>SI-18M1:CO-Counter-Ch4</v>
       </c>
       <c r="I70" s="40" t="str">
         <f>_xlfn.CONCAT($D70,"-Ch5")</f>
-        <v>SI-18M2:CO-Counter-Ch5</v>
+        <v>SI-18M1:CO-Counter-Ch5</v>
       </c>
       <c r="J70" s="40" t="str">
         <f>_xlfn.CONCAT($D70,"-Ch6")</f>
-        <v>SI-18M2:CO-Counter-Ch6</v>
+        <v>SI-18M1:CO-Counter-Ch6</v>
       </c>
       <c r="K70" s="40" t="str">
         <f>_xlfn.CONCAT($D70,"-Ch7")</f>
-        <v>SI-18M2:CO-Counter-Ch7</v>
+        <v>SI-18M1:CO-Counter-Ch7</v>
       </c>
       <c r="L70" s="40" t="str">
         <f>_xlfn.CONCAT($D70,"-Ch8")</f>
-        <v>SI-18M2:CO-Counter-Ch8</v>
+        <v>SI-18M1:CO-Counter-Ch8</v>
       </c>
       <c r="M70" t="s">
         <v>2090</v>
@@ -21582,8 +21594,9 @@
       <c r="T70" t="s">
         <v>2097</v>
       </c>
-      <c r="U70" t="s">
-        <v>2098</v>
+      <c r="U70" t="str">
+        <f>_xlfn.CONCAT("SI-",$C70+1,"M1:CO-GammaDetector")</f>
+        <v>SI-18M1:CO-GammaDetector</v>
       </c>
       <c r="V70" t="s">
         <v>2098</v>
@@ -21591,7 +21604,7 @@
       <c r="W70" t="s">
         <v>2098</v>
       </c>
-      <c r="X70" t="s">
+      <c r="X70" s="40" t="s">
         <v>2098</v>
       </c>
       <c r="Y70" t="s">
@@ -21607,52 +21620,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="71" spans="1:28">
+    <row r="71" spans="1:28" hidden="1">
       <c r="A71" s="93" t="s">
-        <v>30</v>
+        <v>1046</v>
       </c>
       <c r="B71" t="str">
-        <f>_xlfn.CONCAT("10.128.",C71 + 100,".152")</f>
-        <v>10.128.118.152</v>
+        <f>_xlfn.CONCAT("10.128.",C71 + 100,".151")</f>
+        <v>10.128.118.151</v>
       </c>
       <c r="C71" s="65">
         <v>18</v>
       </c>
       <c r="D71" t="str">
-        <f>_xlfn.CONCAT("SI-",C71,"C2:CO-Counter")</f>
-        <v>SI-18C2:CO-Counter</v>
-      </c>
-      <c r="E71" t="str">
-        <f>_xlfn.CONCAT("SI-",$C71,"M2:CO-Gamma")</f>
-        <v>SI-18M2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",C71,"M2:CO-Counter")</f>
+        <v>SI-18M2:CO-Counter</v>
+      </c>
+      <c r="E71" s="40" t="str">
+        <f>_xlfn.CONCAT($D71,":Ch1")</f>
+        <v>SI-18M2:CO-Counter:Ch1</v>
       </c>
       <c r="F71" s="40" t="str">
         <f>_xlfn.CONCAT($D71,"-Ch2")</f>
-        <v>SI-18C2:CO-Counter-Ch2</v>
+        <v>SI-18M2:CO-Counter-Ch2</v>
       </c>
       <c r="G71" s="40" t="str">
         <f>_xlfn.CONCAT($D71,"-Ch3")</f>
-        <v>SI-18C2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H71" t="str">
-        <f>_xlfn.CONCAT("SI-",$C71,"C1:CO-Gamma")</f>
-        <v>SI-18C1:CO-Gamma</v>
+        <v>SI-18M2:CO-Counter-Ch3</v>
+      </c>
+      <c r="H71" s="40" t="str">
+        <f>_xlfn.CONCAT($D71,":Ch4")</f>
+        <v>SI-18M2:CO-Counter:Ch4</v>
       </c>
       <c r="I71" s="40" t="str">
         <f>_xlfn.CONCAT($D71,"-Ch5")</f>
-        <v>SI-18C2:CO-Counter-Ch5</v>
+        <v>SI-18M2:CO-Counter-Ch5</v>
       </c>
       <c r="J71" s="40" t="str">
         <f>_xlfn.CONCAT($D71,"-Ch6")</f>
-        <v>SI-18C2:CO-Counter-Ch6</v>
+        <v>SI-18M2:CO-Counter-Ch6</v>
       </c>
       <c r="K71" s="40" t="str">
         <f>_xlfn.CONCAT($D71,"-Ch7")</f>
-        <v>SI-18C2:CO-Counter-Ch7</v>
+        <v>SI-18M2:CO-Counter-Ch7</v>
       </c>
       <c r="L71" s="40" t="str">
         <f>_xlfn.CONCAT($D71,"-Ch8")</f>
-        <v>SI-18C2:CO-Counter-Ch8</v>
+        <v>SI-18M2:CO-Counter-Ch8</v>
       </c>
       <c r="M71" t="s">
         <v>2090</v>
@@ -21678,9 +21691,8 @@
       <c r="T71" t="s">
         <v>2097</v>
       </c>
-      <c r="U71" t="str">
-        <f>_xlfn.CONCAT("SI-",$C71,"C1:CO-GammaDetector")</f>
-        <v>SI-18C1:CO-GammaDetector</v>
+      <c r="U71" t="s">
+        <v>2098</v>
       </c>
       <c r="V71" t="s">
         <v>2098</v>
@@ -21688,9 +21700,8 @@
       <c r="W71" t="s">
         <v>2098</v>
       </c>
-      <c r="X71" t="str">
-        <f>_xlfn.CONCAT("SI-",$C71,"C2:CO-GammaDetector")</f>
-        <v>SI-18C2:CO-GammaDetector</v>
+      <c r="X71" t="s">
+        <v>2098</v>
       </c>
       <c r="Y71" t="s">
         <v>2098</v>
@@ -21710,47 +21721,47 @@
         <v>30</v>
       </c>
       <c r="B72" t="str">
-        <f>_xlfn.CONCAT("10.128.",C72 + 100,".153")</f>
-        <v>10.128.118.153</v>
+        <f>_xlfn.CONCAT("10.128.",C72 + 100,".152")</f>
+        <v>10.128.118.152</v>
       </c>
       <c r="C72" s="65">
         <v>18</v>
       </c>
       <c r="D72" t="str">
-        <f>_xlfn.CONCAT("SI-",C72,"C3:CO-Counter")</f>
-        <v>SI-18C3:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C72,"C2:CO-Counter")</f>
+        <v>SI-18C2:CO-Counter</v>
       </c>
       <c r="E72" t="str">
-        <f>_xlfn.CONCAT("SI-",$C72,"C2:CO-Gamma")</f>
-        <v>SI-18C2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C72,"M2:CO-Gamma")</f>
+        <v>SI-18M2:CO-Gamma</v>
       </c>
       <c r="F72" s="40" t="str">
         <f>_xlfn.CONCAT($D72,"-Ch2")</f>
-        <v>SI-18C3:CO-Counter-Ch2</v>
+        <v>SI-18C2:CO-Counter-Ch2</v>
       </c>
       <c r="G72" s="40" t="str">
         <f>_xlfn.CONCAT($D72,"-Ch3")</f>
-        <v>SI-18C3:CO-Counter-Ch3</v>
+        <v>SI-18C2:CO-Counter-Ch3</v>
       </c>
       <c r="H72" t="str">
-        <f>_xlfn.CONCAT("SI-",$C72,"C3:CO-Gamma")</f>
-        <v>SI-18C3:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C72,"C1:CO-Gamma")</f>
+        <v>SI-18C1:CO-Gamma</v>
       </c>
       <c r="I72" s="40" t="str">
         <f>_xlfn.CONCAT($D72,"-Ch5")</f>
-        <v>SI-18C3:CO-Counter-Ch5</v>
+        <v>SI-18C2:CO-Counter-Ch5</v>
       </c>
       <c r="J72" s="40" t="str">
         <f>_xlfn.CONCAT($D72,"-Ch6")</f>
-        <v>SI-18C3:CO-Counter-Ch6</v>
+        <v>SI-18C2:CO-Counter-Ch6</v>
       </c>
       <c r="K72" s="40" t="str">
         <f>_xlfn.CONCAT($D72,"-Ch7")</f>
-        <v>SI-18C3:CO-Counter-Ch7</v>
+        <v>SI-18C2:CO-Counter-Ch7</v>
       </c>
       <c r="L72" s="40" t="str">
         <f>_xlfn.CONCAT($D72,"-Ch8")</f>
-        <v>SI-18C3:CO-Counter-Ch8</v>
+        <v>SI-18C2:CO-Counter-Ch8</v>
       </c>
       <c r="M72" t="s">
         <v>2090</v>
@@ -21777,8 +21788,8 @@
         <v>2097</v>
       </c>
       <c r="U72" t="str">
-        <f>_xlfn.CONCAT("SI-",$C72,"C3:CO-GammaDetector")</f>
-        <v>SI-18C3:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C72,"C1:CO-GammaDetector")</f>
+        <v>SI-18C1:CO-GammaDetector</v>
       </c>
       <c r="V72" t="s">
         <v>2098</v>
@@ -21787,8 +21798,8 @@
         <v>2098</v>
       </c>
       <c r="X72" t="str">
-        <f>_xlfn.CONCAT("SI-",$C72,"C4:CO-GammaDetector")</f>
-        <v>SI-18C4:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C72,"C2:CO-GammaDetector")</f>
+        <v>SI-18C2:CO-GammaDetector</v>
       </c>
       <c r="Y72" t="s">
         <v>2098</v>
@@ -21808,47 +21819,47 @@
         <v>30</v>
       </c>
       <c r="B73" t="str">
-        <f>_xlfn.CONCAT("10.128.",C73 + 100,".154")</f>
-        <v>10.128.118.154</v>
+        <f>_xlfn.CONCAT("10.128.",C73 + 100,".153")</f>
+        <v>10.128.118.153</v>
       </c>
       <c r="C73" s="65">
         <v>18</v>
       </c>
       <c r="D73" t="str">
-        <f>_xlfn.CONCAT("SI-",C73+1,"M1:CO-Counter")</f>
-        <v>SI-19M1:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C73,"C3:CO-Counter")</f>
+        <v>SI-18C3:CO-Counter</v>
       </c>
       <c r="E73" t="str">
-        <f>_xlfn.CONCAT("SI-",$C73,"C4:CO-Gamma")</f>
-        <v>SI-18C4:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C73,"C2:CO-Gamma")</f>
+        <v>SI-18C2:CO-Gamma</v>
       </c>
       <c r="F73" s="40" t="str">
         <f>_xlfn.CONCAT($D73,"-Ch2")</f>
-        <v>SI-19M1:CO-Counter-Ch2</v>
+        <v>SI-18C3:CO-Counter-Ch2</v>
       </c>
       <c r="G73" s="40" t="str">
         <f>_xlfn.CONCAT($D73,"-Ch3")</f>
-        <v>SI-19M1:CO-Counter-Ch3</v>
-      </c>
-      <c r="H73" s="40" t="str">
-        <f>_xlfn.CONCAT($D73,"-Ch4")</f>
-        <v>SI-19M1:CO-Counter-Ch4</v>
+        <v>SI-18C3:CO-Counter-Ch3</v>
+      </c>
+      <c r="H73" t="str">
+        <f>_xlfn.CONCAT("SI-",$C73,"C3:CO-Gamma")</f>
+        <v>SI-18C3:CO-Gamma</v>
       </c>
       <c r="I73" s="40" t="str">
         <f>_xlfn.CONCAT($D73,"-Ch5")</f>
-        <v>SI-19M1:CO-Counter-Ch5</v>
+        <v>SI-18C3:CO-Counter-Ch5</v>
       </c>
       <c r="J73" s="40" t="str">
         <f>_xlfn.CONCAT($D73,"-Ch6")</f>
-        <v>SI-19M1:CO-Counter-Ch6</v>
+        <v>SI-18C3:CO-Counter-Ch6</v>
       </c>
       <c r="K73" s="40" t="str">
         <f>_xlfn.CONCAT($D73,"-Ch7")</f>
-        <v>SI-19M1:CO-Counter-Ch7</v>
+        <v>SI-18C3:CO-Counter-Ch7</v>
       </c>
       <c r="L73" s="40" t="str">
         <f>_xlfn.CONCAT($D73,"-Ch8")</f>
-        <v>SI-19M1:CO-Counter-Ch8</v>
+        <v>SI-18C3:CO-Counter-Ch8</v>
       </c>
       <c r="M73" t="s">
         <v>2090</v>
@@ -21875,8 +21886,8 @@
         <v>2097</v>
       </c>
       <c r="U73" t="str">
-        <f>_xlfn.CONCAT("SI-",$C73+1,"M1:CO-GammaDetector")</f>
-        <v>SI-19M1:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C73,"C3:CO-GammaDetector")</f>
+        <v>SI-18C3:CO-GammaDetector</v>
       </c>
       <c r="V73" t="s">
         <v>2098</v>
@@ -21884,8 +21895,9 @@
       <c r="W73" t="s">
         <v>2098</v>
       </c>
-      <c r="X73" s="40" t="s">
-        <v>2098</v>
+      <c r="X73" t="str">
+        <f>_xlfn.CONCAT("SI-",$C73,"C4:CO-GammaDetector")</f>
+        <v>SI-18C4:CO-GammaDetector</v>
       </c>
       <c r="Y73" t="s">
         <v>2098</v>
@@ -21900,52 +21912,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="74" spans="1:28" hidden="1">
+    <row r="74" spans="1:28">
       <c r="A74" s="93" t="s">
-        <v>1046</v>
+        <v>30</v>
       </c>
       <c r="B74" t="str">
-        <f>_xlfn.CONCAT("10.128.",C74 + 100,".151")</f>
-        <v>10.128.119.151</v>
+        <f>_xlfn.CONCAT("10.128.",C74 + 100,".154")</f>
+        <v>10.128.118.154</v>
       </c>
       <c r="C74" s="65">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D74" t="str">
-        <f>_xlfn.CONCAT("SI-",C74,"M2:CO-Counter")</f>
-        <v>SI-19M2:CO-Counter</v>
-      </c>
-      <c r="E74" s="40" t="str">
-        <f>_xlfn.CONCAT($D74,":Ch1")</f>
-        <v>SI-19M2:CO-Counter:Ch1</v>
+        <f>_xlfn.CONCAT("SI-",C74+1,"M1:CO-Counter")</f>
+        <v>SI-19M1:CO-Counter</v>
+      </c>
+      <c r="E74" t="str">
+        <f>_xlfn.CONCAT("SI-",$C74,"C4:CO-Gamma")</f>
+        <v>SI-18C4:CO-Gamma</v>
       </c>
       <c r="F74" s="40" t="str">
         <f>_xlfn.CONCAT($D74,"-Ch2")</f>
-        <v>SI-19M2:CO-Counter-Ch2</v>
+        <v>SI-19M1:CO-Counter-Ch2</v>
       </c>
       <c r="G74" s="40" t="str">
         <f>_xlfn.CONCAT($D74,"-Ch3")</f>
-        <v>SI-19M2:CO-Counter-Ch3</v>
+        <v>SI-19M1:CO-Counter-Ch3</v>
       </c>
       <c r="H74" s="40" t="str">
-        <f>_xlfn.CONCAT($D74,":Ch4")</f>
-        <v>SI-19M2:CO-Counter:Ch4</v>
+        <f>_xlfn.CONCAT($D74,"-Ch4")</f>
+        <v>SI-19M1:CO-Counter-Ch4</v>
       </c>
       <c r="I74" s="40" t="str">
         <f>_xlfn.CONCAT($D74,"-Ch5")</f>
-        <v>SI-19M2:CO-Counter-Ch5</v>
+        <v>SI-19M1:CO-Counter-Ch5</v>
       </c>
       <c r="J74" s="40" t="str">
         <f>_xlfn.CONCAT($D74,"-Ch6")</f>
-        <v>SI-19M2:CO-Counter-Ch6</v>
+        <v>SI-19M1:CO-Counter-Ch6</v>
       </c>
       <c r="K74" s="40" t="str">
         <f>_xlfn.CONCAT($D74,"-Ch7")</f>
-        <v>SI-19M2:CO-Counter-Ch7</v>
+        <v>SI-19M1:CO-Counter-Ch7</v>
       </c>
       <c r="L74" s="40" t="str">
         <f>_xlfn.CONCAT($D74,"-Ch8")</f>
-        <v>SI-19M2:CO-Counter-Ch8</v>
+        <v>SI-19M1:CO-Counter-Ch8</v>
       </c>
       <c r="M74" t="s">
         <v>2090</v>
@@ -21971,8 +21983,9 @@
       <c r="T74" t="s">
         <v>2097</v>
       </c>
-      <c r="U74" t="s">
-        <v>2098</v>
+      <c r="U74" t="str">
+        <f>_xlfn.CONCAT("SI-",$C74+1,"M1:CO-GammaDetector")</f>
+        <v>SI-19M1:CO-GammaDetector</v>
       </c>
       <c r="V74" t="s">
         <v>2098</v>
@@ -21980,7 +21993,7 @@
       <c r="W74" t="s">
         <v>2098</v>
       </c>
-      <c r="X74" t="s">
+      <c r="X74" s="40" t="s">
         <v>2098</v>
       </c>
       <c r="Y74" t="s">
@@ -21996,52 +22009,52 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="75" spans="1:28">
+    <row r="75" spans="1:28" hidden="1">
       <c r="A75" s="93" t="s">
-        <v>30</v>
+        <v>1046</v>
       </c>
       <c r="B75" t="str">
-        <f>_xlfn.CONCAT("10.128.",C75 + 100,".152")</f>
-        <v>10.128.119.152</v>
+        <f>_xlfn.CONCAT("10.128.",C75 + 100,".151")</f>
+        <v>10.128.119.151</v>
       </c>
       <c r="C75" s="65">
         <v>19</v>
       </c>
       <c r="D75" t="str">
-        <f>_xlfn.CONCAT("SI-",C75,"C2:CO-Counter")</f>
-        <v>SI-19C2:CO-Counter</v>
-      </c>
-      <c r="E75" t="str">
-        <f>_xlfn.CONCAT("SI-",$C75,"M2:CO-Gamma")</f>
-        <v>SI-19M2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",C75,"M2:CO-Counter")</f>
+        <v>SI-19M2:CO-Counter</v>
+      </c>
+      <c r="E75" s="40" t="str">
+        <f>_xlfn.CONCAT($D75,":Ch1")</f>
+        <v>SI-19M2:CO-Counter:Ch1</v>
       </c>
       <c r="F75" s="40" t="str">
         <f>_xlfn.CONCAT($D75,"-Ch2")</f>
-        <v>SI-19C2:CO-Counter-Ch2</v>
+        <v>SI-19M2:CO-Counter-Ch2</v>
       </c>
       <c r="G75" s="40" t="str">
         <f>_xlfn.CONCAT($D75,"-Ch3")</f>
-        <v>SI-19C2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H75" t="str">
-        <f>_xlfn.CONCAT("SI-",$C75,"C1:CO-Gamma")</f>
-        <v>SI-19C1:CO-Gamma</v>
+        <v>SI-19M2:CO-Counter-Ch3</v>
+      </c>
+      <c r="H75" s="40" t="str">
+        <f>_xlfn.CONCAT($D75,":Ch4")</f>
+        <v>SI-19M2:CO-Counter:Ch4</v>
       </c>
       <c r="I75" s="40" t="str">
         <f>_xlfn.CONCAT($D75,"-Ch5")</f>
-        <v>SI-19C2:CO-Counter-Ch5</v>
+        <v>SI-19M2:CO-Counter-Ch5</v>
       </c>
       <c r="J75" s="40" t="str">
         <f>_xlfn.CONCAT($D75,"-Ch6")</f>
-        <v>SI-19C2:CO-Counter-Ch6</v>
+        <v>SI-19M2:CO-Counter-Ch6</v>
       </c>
       <c r="K75" s="40" t="str">
         <f>_xlfn.CONCAT($D75,"-Ch7")</f>
-        <v>SI-19C2:CO-Counter-Ch7</v>
+        <v>SI-19M2:CO-Counter-Ch7</v>
       </c>
       <c r="L75" s="40" t="str">
         <f>_xlfn.CONCAT($D75,"-Ch8")</f>
-        <v>SI-19C2:CO-Counter-Ch8</v>
+        <v>SI-19M2:CO-Counter-Ch8</v>
       </c>
       <c r="M75" t="s">
         <v>2090</v>
@@ -22067,9 +22080,8 @@
       <c r="T75" t="s">
         <v>2097</v>
       </c>
-      <c r="U75" t="str">
-        <f>_xlfn.CONCAT("SI-",$C75,"C1:CO-GammaDetector")</f>
-        <v>SI-19C1:CO-GammaDetector</v>
+      <c r="U75" t="s">
+        <v>2098</v>
       </c>
       <c r="V75" t="s">
         <v>2098</v>
@@ -22077,9 +22089,8 @@
       <c r="W75" t="s">
         <v>2098</v>
       </c>
-      <c r="X75" t="str">
-        <f>_xlfn.CONCAT("SI-",$C75,"C2:CO-GammaDetector")</f>
-        <v>SI-19C2:CO-GammaDetector</v>
+      <c r="X75" t="s">
+        <v>2098</v>
       </c>
       <c r="Y75" t="s">
         <v>2098</v>
@@ -22099,47 +22110,47 @@
         <v>30</v>
       </c>
       <c r="B76" t="str">
-        <f>_xlfn.CONCAT("10.128.",C76 + 100,".153")</f>
-        <v>10.128.119.153</v>
+        <f>_xlfn.CONCAT("10.128.",C76 + 100,".152")</f>
+        <v>10.128.119.152</v>
       </c>
       <c r="C76" s="65">
         <v>19</v>
       </c>
       <c r="D76" t="str">
-        <f>_xlfn.CONCAT("SI-",C76,"C3:CO-Counter")</f>
-        <v>SI-19C3:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C76,"C2:CO-Counter")</f>
+        <v>SI-19C2:CO-Counter</v>
       </c>
       <c r="E76" t="str">
-        <f>_xlfn.CONCAT("SI-",$C76,"C2:CO-Gamma")</f>
-        <v>SI-19C2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C76,"M2:CO-Gamma")</f>
+        <v>SI-19M2:CO-Gamma</v>
       </c>
       <c r="F76" s="40" t="str">
         <f>_xlfn.CONCAT($D76,"-Ch2")</f>
-        <v>SI-19C3:CO-Counter-Ch2</v>
+        <v>SI-19C2:CO-Counter-Ch2</v>
       </c>
       <c r="G76" s="40" t="str">
         <f>_xlfn.CONCAT($D76,"-Ch3")</f>
-        <v>SI-19C3:CO-Counter-Ch3</v>
+        <v>SI-19C2:CO-Counter-Ch3</v>
       </c>
       <c r="H76" t="str">
-        <f>_xlfn.CONCAT("SI-",$C76,"C3:CO-Gamma")</f>
-        <v>SI-19C3:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C76,"C1:CO-Gamma")</f>
+        <v>SI-19C1:CO-Gamma</v>
       </c>
       <c r="I76" s="40" t="str">
         <f>_xlfn.CONCAT($D76,"-Ch5")</f>
-        <v>SI-19C3:CO-Counter-Ch5</v>
+        <v>SI-19C2:CO-Counter-Ch5</v>
       </c>
       <c r="J76" s="40" t="str">
         <f>_xlfn.CONCAT($D76,"-Ch6")</f>
-        <v>SI-19C3:CO-Counter-Ch6</v>
+        <v>SI-19C2:CO-Counter-Ch6</v>
       </c>
       <c r="K76" s="40" t="str">
         <f>_xlfn.CONCAT($D76,"-Ch7")</f>
-        <v>SI-19C3:CO-Counter-Ch7</v>
+        <v>SI-19C2:CO-Counter-Ch7</v>
       </c>
       <c r="L76" s="40" t="str">
         <f>_xlfn.CONCAT($D76,"-Ch8")</f>
-        <v>SI-19C3:CO-Counter-Ch8</v>
+        <v>SI-19C2:CO-Counter-Ch8</v>
       </c>
       <c r="M76" t="s">
         <v>2090</v>
@@ -22166,8 +22177,8 @@
         <v>2097</v>
       </c>
       <c r="U76" t="str">
-        <f>_xlfn.CONCAT("SI-",$C76,"C3:CO-GammaDetector")</f>
-        <v>SI-19C3:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C76,"C1:CO-GammaDetector")</f>
+        <v>SI-19C1:CO-GammaDetector</v>
       </c>
       <c r="V76" t="s">
         <v>2098</v>
@@ -22176,8 +22187,8 @@
         <v>2098</v>
       </c>
       <c r="X76" t="str">
-        <f>_xlfn.CONCAT("SI-",$C76,"C4:CO-GammaDetector")</f>
-        <v>SI-19C4:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C76,"C2:CO-GammaDetector")</f>
+        <v>SI-19C2:CO-GammaDetector</v>
       </c>
       <c r="Y76" t="s">
         <v>2098</v>
@@ -22197,47 +22208,47 @@
         <v>30</v>
       </c>
       <c r="B77" t="str">
-        <f>_xlfn.CONCAT("10.128.",C77 + 100,".154")</f>
-        <v>10.128.119.154</v>
+        <f>_xlfn.CONCAT("10.128.",C77 + 100,".153")</f>
+        <v>10.128.119.153</v>
       </c>
       <c r="C77" s="65">
         <v>19</v>
       </c>
       <c r="D77" t="str">
-        <f>_xlfn.CONCAT("SI-",C77+1,"M1:CO-Counter")</f>
-        <v>SI-20M1:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C77,"C3:CO-Counter")</f>
+        <v>SI-19C3:CO-Counter</v>
       </c>
       <c r="E77" t="str">
-        <f>_xlfn.CONCAT("SI-",$C77,"C4:CO-Gamma")</f>
-        <v>SI-19C4:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C77,"C2:CO-Gamma")</f>
+        <v>SI-19C2:CO-Gamma</v>
       </c>
       <c r="F77" s="40" t="str">
         <f>_xlfn.CONCAT($D77,"-Ch2")</f>
-        <v>SI-20M1:CO-Counter-Ch2</v>
+        <v>SI-19C3:CO-Counter-Ch2</v>
       </c>
       <c r="G77" s="40" t="str">
         <f>_xlfn.CONCAT($D77,"-Ch3")</f>
-        <v>SI-20M1:CO-Counter-Ch3</v>
-      </c>
-      <c r="H77" s="40" t="str">
-        <f>_xlfn.CONCAT($D77,"-Ch4")</f>
-        <v>SI-20M1:CO-Counter-Ch4</v>
+        <v>SI-19C3:CO-Counter-Ch3</v>
+      </c>
+      <c r="H77" t="str">
+        <f>_xlfn.CONCAT("SI-",$C77,"C3:CO-Gamma")</f>
+        <v>SI-19C3:CO-Gamma</v>
       </c>
       <c r="I77" s="40" t="str">
         <f>_xlfn.CONCAT($D77,"-Ch5")</f>
-        <v>SI-20M1:CO-Counter-Ch5</v>
+        <v>SI-19C3:CO-Counter-Ch5</v>
       </c>
       <c r="J77" s="40" t="str">
         <f>_xlfn.CONCAT($D77,"-Ch6")</f>
-        <v>SI-20M1:CO-Counter-Ch6</v>
+        <v>SI-19C3:CO-Counter-Ch6</v>
       </c>
       <c r="K77" s="40" t="str">
         <f>_xlfn.CONCAT($D77,"-Ch7")</f>
-        <v>SI-20M1:CO-Counter-Ch7</v>
+        <v>SI-19C3:CO-Counter-Ch7</v>
       </c>
       <c r="L77" s="40" t="str">
         <f>_xlfn.CONCAT($D77,"-Ch8")</f>
-        <v>SI-20M1:CO-Counter-Ch8</v>
+        <v>SI-19C3:CO-Counter-Ch8</v>
       </c>
       <c r="M77" t="s">
         <v>2090</v>
@@ -22264,8 +22275,8 @@
         <v>2097</v>
       </c>
       <c r="U77" t="str">
-        <f>_xlfn.CONCAT("SI-",$C77+1,"M1:CO-GammaDetector")</f>
-        <v>SI-20M1:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C77,"C3:CO-GammaDetector")</f>
+        <v>SI-19C3:CO-GammaDetector</v>
       </c>
       <c r="V77" t="s">
         <v>2098</v>
@@ -22273,8 +22284,9 @@
       <c r="W77" t="s">
         <v>2098</v>
       </c>
-      <c r="X77" s="40" t="s">
-        <v>2098</v>
+      <c r="X77" t="str">
+        <f>_xlfn.CONCAT("SI-",$C77,"C4:CO-GammaDetector")</f>
+        <v>SI-19C4:CO-GammaDetector</v>
       </c>
       <c r="Y77" t="s">
         <v>2098</v>
@@ -22294,47 +22306,47 @@
         <v>30</v>
       </c>
       <c r="B78" t="str">
-        <f>_xlfn.CONCAT("10.128.",C78 + 100,".152")</f>
-        <v>10.128.120.152</v>
+        <f>_xlfn.CONCAT("10.128.",C78 + 100,".154")</f>
+        <v>10.128.119.154</v>
       </c>
       <c r="C78" s="65">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78" t="str">
-        <f>_xlfn.CONCAT("SI-",C78,"C2:CO-Counter")</f>
-        <v>SI-20C2:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C78+1,"M1:CO-Counter")</f>
+        <v>SI-20M1:CO-Counter</v>
       </c>
       <c r="E78" t="str">
-        <f>_xlfn.CONCAT("SI-",$C78,"M2:CO-Gamma")</f>
-        <v>SI-20M2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C78,"C4:CO-Gamma")</f>
+        <v>SI-19C4:CO-Gamma</v>
       </c>
       <c r="F78" s="40" t="str">
         <f>_xlfn.CONCAT($D78,"-Ch2")</f>
-        <v>SI-20C2:CO-Counter-Ch2</v>
+        <v>SI-20M1:CO-Counter-Ch2</v>
       </c>
       <c r="G78" s="40" t="str">
         <f>_xlfn.CONCAT($D78,"-Ch3")</f>
-        <v>SI-20C2:CO-Counter-Ch3</v>
-      </c>
-      <c r="H78" t="str">
-        <f>_xlfn.CONCAT("SI-",$C78,"C1:CO-Gamma")</f>
-        <v>SI-20C1:CO-Gamma</v>
+        <v>SI-20M1:CO-Counter-Ch3</v>
+      </c>
+      <c r="H78" s="40" t="str">
+        <f>_xlfn.CONCAT($D78,"-Ch4")</f>
+        <v>SI-20M1:CO-Counter-Ch4</v>
       </c>
       <c r="I78" s="40" t="str">
         <f>_xlfn.CONCAT($D78,"-Ch5")</f>
-        <v>SI-20C2:CO-Counter-Ch5</v>
+        <v>SI-20M1:CO-Counter-Ch5</v>
       </c>
       <c r="J78" s="40" t="str">
         <f>_xlfn.CONCAT($D78,"-Ch6")</f>
-        <v>SI-20C2:CO-Counter-Ch6</v>
+        <v>SI-20M1:CO-Counter-Ch6</v>
       </c>
       <c r="K78" s="40" t="str">
         <f>_xlfn.CONCAT($D78,"-Ch7")</f>
-        <v>SI-20C2:CO-Counter-Ch7</v>
+        <v>SI-20M1:CO-Counter-Ch7</v>
       </c>
       <c r="L78" s="40" t="str">
         <f>_xlfn.CONCAT($D78,"-Ch8")</f>
-        <v>SI-20C2:CO-Counter-Ch8</v>
+        <v>SI-20M1:CO-Counter-Ch8</v>
       </c>
       <c r="M78" t="s">
         <v>2090</v>
@@ -22361,8 +22373,8 @@
         <v>2097</v>
       </c>
       <c r="U78" t="str">
-        <f>_xlfn.CONCAT("SI-",$C78,"C1:CO-GammaDetector")</f>
-        <v>SI-20C1:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C78+1,"M1:CO-GammaDetector")</f>
+        <v>SI-20M1:CO-GammaDetector</v>
       </c>
       <c r="V78" t="s">
         <v>2098</v>
@@ -22370,9 +22382,8 @@
       <c r="W78" t="s">
         <v>2098</v>
       </c>
-      <c r="X78" t="str">
-        <f>_xlfn.CONCAT("SI-",$C78,"C2:CO-GammaDetector")</f>
-        <v>SI-20C2:CO-GammaDetector</v>
+      <c r="X78" s="40" t="s">
+        <v>2098</v>
       </c>
       <c r="Y78" t="s">
         <v>2098</v>
@@ -22392,47 +22403,47 @@
         <v>30</v>
       </c>
       <c r="B79" t="str">
-        <f>_xlfn.CONCAT("10.128.",C79 + 100,".153")</f>
-        <v>10.128.120.153</v>
+        <f>_xlfn.CONCAT("10.128.",C79 + 100,".152")</f>
+        <v>10.128.120.152</v>
       </c>
       <c r="C79" s="65">
         <v>20</v>
       </c>
       <c r="D79" t="str">
-        <f>_xlfn.CONCAT("SI-",C79,"C3:CO-Counter")</f>
-        <v>SI-20C3:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C79,"C2:CO-Counter")</f>
+        <v>SI-20C2:CO-Counter</v>
       </c>
       <c r="E79" t="str">
-        <f>_xlfn.CONCAT("SI-",$C79,"C2:CO-Gamma")</f>
-        <v>SI-20C2:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C79,"M2:CO-Gamma")</f>
+        <v>SI-20M2:CO-Gamma</v>
       </c>
       <c r="F79" s="40" t="str">
         <f>_xlfn.CONCAT($D79,"-Ch2")</f>
-        <v>SI-20C3:CO-Counter-Ch2</v>
+        <v>SI-20C2:CO-Counter-Ch2</v>
       </c>
       <c r="G79" s="40" t="str">
         <f>_xlfn.CONCAT($D79,"-Ch3")</f>
-        <v>SI-20C3:CO-Counter-Ch3</v>
+        <v>SI-20C2:CO-Counter-Ch3</v>
       </c>
       <c r="H79" t="str">
-        <f>_xlfn.CONCAT("SI-",$C79,"C3:CO-Gamma")</f>
-        <v>SI-20C3:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C79,"C1:CO-Gamma")</f>
+        <v>SI-20C1:CO-Gamma</v>
       </c>
       <c r="I79" s="40" t="str">
         <f>_xlfn.CONCAT($D79,"-Ch5")</f>
-        <v>SI-20C3:CO-Counter-Ch5</v>
+        <v>SI-20C2:CO-Counter-Ch5</v>
       </c>
       <c r="J79" s="40" t="str">
         <f>_xlfn.CONCAT($D79,"-Ch6")</f>
-        <v>SI-20C3:CO-Counter-Ch6</v>
+        <v>SI-20C2:CO-Counter-Ch6</v>
       </c>
       <c r="K79" s="40" t="str">
         <f>_xlfn.CONCAT($D79,"-Ch7")</f>
-        <v>SI-20C3:CO-Counter-Ch7</v>
+        <v>SI-20C2:CO-Counter-Ch7</v>
       </c>
       <c r="L79" s="40" t="str">
         <f>_xlfn.CONCAT($D79,"-Ch8")</f>
-        <v>SI-20C3:CO-Counter-Ch8</v>
+        <v>SI-20C2:CO-Counter-Ch8</v>
       </c>
       <c r="M79" t="s">
         <v>2090</v>
@@ -22459,8 +22470,8 @@
         <v>2097</v>
       </c>
       <c r="U79" t="str">
-        <f>_xlfn.CONCAT("SI-",$C79,"C3:CO-GammaDetector")</f>
-        <v>SI-20C3:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C79,"C1:CO-GammaDetector")</f>
+        <v>SI-20C1:CO-GammaDetector</v>
       </c>
       <c r="V79" t="s">
         <v>2098</v>
@@ -22469,8 +22480,8 @@
         <v>2098</v>
       </c>
       <c r="X79" t="str">
-        <f>_xlfn.CONCAT("SI-",$C79,"C4:CO-GammaDetector")</f>
-        <v>SI-20C4:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C79,"C2:CO-GammaDetector")</f>
+        <v>SI-20C2:CO-GammaDetector</v>
       </c>
       <c r="Y79" t="s">
         <v>2098</v>
@@ -22490,47 +22501,47 @@
         <v>30</v>
       </c>
       <c r="B80" t="str">
-        <f>_xlfn.CONCAT("10.128.",C80 + 100,".154")</f>
-        <v>10.128.120.154</v>
+        <f>_xlfn.CONCAT("10.128.",C80 + 100,".153")</f>
+        <v>10.128.120.153</v>
       </c>
       <c r="C80" s="65">
         <v>20</v>
       </c>
       <c r="D80" t="str">
-        <f>_xlfn.CONCAT("SI-0",C80-19,"M1:CO-Counter")</f>
-        <v>SI-01M1:CO-Counter</v>
+        <f>_xlfn.CONCAT("SI-",C80,"C3:CO-Counter")</f>
+        <v>SI-20C3:CO-Counter</v>
       </c>
       <c r="E80" t="str">
-        <f>_xlfn.CONCAT("SI-",$C80,"C4:CO-Gamma")</f>
-        <v>SI-20C4:CO-Gamma</v>
+        <f>_xlfn.CONCAT("SI-",$C80,"C2:CO-Gamma")</f>
+        <v>SI-20C2:CO-Gamma</v>
       </c>
       <c r="F80" s="40" t="str">
         <f>_xlfn.CONCAT($D80,"-Ch2")</f>
-        <v>SI-01M1:CO-Counter-Ch2</v>
+        <v>SI-20C3:CO-Counter-Ch2</v>
       </c>
       <c r="G80" s="40" t="str">
         <f>_xlfn.CONCAT($D80,"-Ch3")</f>
-        <v>SI-01M1:CO-Counter-Ch3</v>
-      </c>
-      <c r="H80" s="40" t="str">
-        <f>_xlfn.CONCAT($D80,"-Ch4")</f>
-        <v>SI-01M1:CO-Counter-Ch4</v>
+        <v>SI-20C3:CO-Counter-Ch3</v>
+      </c>
+      <c r="H80" t="str">
+        <f>_xlfn.CONCAT("SI-",$C80,"C3:CO-Gamma")</f>
+        <v>SI-20C3:CO-Gamma</v>
       </c>
       <c r="I80" s="40" t="str">
         <f>_xlfn.CONCAT($D80,"-Ch5")</f>
-        <v>SI-01M1:CO-Counter-Ch5</v>
+        <v>SI-20C3:CO-Counter-Ch5</v>
       </c>
       <c r="J80" s="40" t="str">
         <f>_xlfn.CONCAT($D80,"-Ch6")</f>
-        <v>SI-01M1:CO-Counter-Ch6</v>
+        <v>SI-20C3:CO-Counter-Ch6</v>
       </c>
       <c r="K80" s="40" t="str">
         <f>_xlfn.CONCAT($D80,"-Ch7")</f>
-        <v>SI-01M1:CO-Counter-Ch7</v>
+        <v>SI-20C3:CO-Counter-Ch7</v>
       </c>
       <c r="L80" s="40" t="str">
         <f>_xlfn.CONCAT($D80,"-Ch8")</f>
-        <v>SI-01M1:CO-Counter-Ch8</v>
+        <v>SI-20C3:CO-Counter-Ch8</v>
       </c>
       <c r="M80" t="s">
         <v>2090</v>
@@ -22557,8 +22568,8 @@
         <v>2097</v>
       </c>
       <c r="U80" t="str">
-        <f>_xlfn.CONCAT("SI-0",$C80-19,"M1:CO-GammaDetector")</f>
-        <v>SI-01M1:CO-GammaDetector</v>
+        <f>_xlfn.CONCAT("SI-",$C80,"C3:CO-GammaDetector")</f>
+        <v>SI-20C3:CO-GammaDetector</v>
       </c>
       <c r="V80" t="s">
         <v>2098</v>
@@ -22566,8 +22577,9 @@
       <c r="W80" t="s">
         <v>2098</v>
       </c>
-      <c r="X80" s="40" t="s">
-        <v>2098</v>
+      <c r="X80" t="str">
+        <f>_xlfn.CONCAT("SI-",$C80,"C4:CO-GammaDetector")</f>
+        <v>SI-20C4:CO-GammaDetector</v>
       </c>
       <c r="Y80" t="s">
         <v>2098</v>
@@ -22582,13 +22594,110 @@
         <v>2098</v>
       </c>
     </row>
+    <row r="81" spans="1:28">
+      <c r="A81" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" t="str">
+        <f>_xlfn.CONCAT("10.128.",C81 + 100,".154")</f>
+        <v>10.128.120.154</v>
+      </c>
+      <c r="C81" s="65">
+        <v>20</v>
+      </c>
+      <c r="D81" t="str">
+        <f>_xlfn.CONCAT("SI-0",C81-19,"M1:CO-Counter")</f>
+        <v>SI-01M1:CO-Counter</v>
+      </c>
+      <c r="E81" t="str">
+        <f>_xlfn.CONCAT("SI-",$C81,"C4:CO-Gamma")</f>
+        <v>SI-20C4:CO-Gamma</v>
+      </c>
+      <c r="F81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch2")</f>
+        <v>SI-01M1:CO-Counter-Ch2</v>
+      </c>
+      <c r="G81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch3")</f>
+        <v>SI-01M1:CO-Counter-Ch3</v>
+      </c>
+      <c r="H81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch4")</f>
+        <v>SI-01M1:CO-Counter-Ch4</v>
+      </c>
+      <c r="I81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch5")</f>
+        <v>SI-01M1:CO-Counter-Ch5</v>
+      </c>
+      <c r="J81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch6")</f>
+        <v>SI-01M1:CO-Counter-Ch6</v>
+      </c>
+      <c r="K81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch7")</f>
+        <v>SI-01M1:CO-Counter-Ch7</v>
+      </c>
+      <c r="L81" s="40" t="str">
+        <f>_xlfn.CONCAT($D81,"-Ch8")</f>
+        <v>SI-01M1:CO-Counter-Ch8</v>
+      </c>
+      <c r="M81" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N81" t="s">
+        <v>2091</v>
+      </c>
+      <c r="O81" t="s">
+        <v>2092</v>
+      </c>
+      <c r="P81" t="s">
+        <v>2093</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>2094</v>
+      </c>
+      <c r="R81" t="s">
+        <v>2095</v>
+      </c>
+      <c r="S81" t="s">
+        <v>2096</v>
+      </c>
+      <c r="T81" t="s">
+        <v>2097</v>
+      </c>
+      <c r="U81" t="str">
+        <f>_xlfn.CONCAT("SI-0",$C81-19,"M1:CO-GammaDetector")</f>
+        <v>SI-01M1:CO-GammaDetector</v>
+      </c>
+      <c r="V81" t="s">
+        <v>2098</v>
+      </c>
+      <c r="W81" t="s">
+        <v>2098</v>
+      </c>
+      <c r="X81" s="40" t="s">
+        <v>2098</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>2098</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>2098</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>2098</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>2098</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:X80" xr:uid="{68EA83DB-34C0-457B-9236-8486C04FD179}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X80">
-      <sortCondition ref="B1:B80"/>
+  <autoFilter ref="A1:X81" xr:uid="{68EA83DB-34C0-457B-9236-8486C04FD179}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X81">
+      <sortCondition ref="B1:B81"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A1 A81:A1048576">
+  <conditionalFormatting sqref="A1 A82:A1048576">
     <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>"True"</formula>
     </cfRule>
@@ -22623,22 +22732,22 @@
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10 A14 A18 A22 A58 A62 A66 A70 A74">
+  <conditionalFormatting sqref="A10 A14 A18 A22 A58 A63 A67 A71 A75">
     <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11 A15 A19 A23 A59 A63 A67 A71 A75 A78:A79">
+  <conditionalFormatting sqref="A11 A15 A19 A23 A59 A64 A68 A72 A76 A79:A80">
     <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12 A16 A20 A24 A60 A64 A68 A72 A76">
+  <conditionalFormatting sqref="A12 A16 A20 A24 A60 A65 A69 A73 A77">
     <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13 A17 A21 A25 A61 A65 A69 A73 A77 A80">
+  <conditionalFormatting sqref="A13 A17 A21 A25 A66 A70 A74 A78 A81 A61:A62">
     <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
       <formula>"True"</formula>
     </cfRule>
@@ -63243,7 +63352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EAC2745-51F2-425B-82EA-1D82E3E9074F}">
   <dimension ref="A1:AE80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" workbookViewId="0">
+    <sheetView topLeftCell="C67" workbookViewId="0">
       <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>

</xml_diff>